<commit_message>
add rd connect structure
</commit_message>
<xml_diff>
--- a/eu_rd_connect.xlsx
+++ b/eu_rd_connect.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" state="visible" r:id="rId2"/>
@@ -319,6 +319,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -340,6 +341,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -554,19 +556,19 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -794,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:AN14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -939,8 +941,12 @@
       <c r="E2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="1" t="b">
+      <c r="G2" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="H2" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +959,11 @@
       <c r="E3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="1" t="b">
+      <c r="G3" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -967,7 +977,11 @@
       <c r="E4" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="1" t="b">
+      <c r="G4" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -981,7 +995,11 @@
       <c r="E5" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="1" t="b">
+      <c r="G5" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -995,7 +1013,11 @@
       <c r="E6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="1" t="b">
+      <c r="G6" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1009,7 +1031,11 @@
       <c r="E7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1" t="b">
+      <c r="G7" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1023,7 +1049,11 @@
       <c r="E8" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="1" t="b">
+      <c r="G8" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1037,7 +1067,11 @@
       <c r="E9" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="1" t="b">
+      <c r="G9" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1051,7 +1085,11 @@
       <c r="E10" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="1" t="b">
+      <c r="G10" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1065,7 +1103,11 @@
       <c r="E11" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="1" t="b">
+      <c r="G11" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1079,7 +1121,11 @@
       <c r="E12" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="1" t="b">
+      <c r="G12" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1093,7 +1139,11 @@
       <c r="E13" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="1" t="b">
+      <c r="G13" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>